<commit_message>
50 simulation for 0M budget
</commit_message>
<xml_diff>
--- a/Results/20231224 Revision_Simulated_Tornado_0M.xlsx
+++ b/Results/20231224 Revision_Simulated_Tornado_0M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E9CADA-AC34-4366-95E0-DC8FF14C2798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BCFCDA-6FF9-4B29-867C-9C3EDE144AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,7 +505,7 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3565,8 +3565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A1BAFE-8EF2-4154-8DC1-44AF14DC1894}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3626,6 +3626,36 @@
       <c r="C2">
         <v>87</v>
       </c>
+      <c r="D2">
+        <v>13088</v>
+      </c>
+      <c r="E2">
+        <v>13088</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>64.33</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>64.2</v>
+      </c>
+      <c r="J2">
+        <v>451</v>
+      </c>
+      <c r="K2">
+        <v>57.06</v>
+      </c>
+      <c r="L2">
+        <v>381</v>
+      </c>
+      <c r="M2">
+        <v>25.43</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -3636,6 +3666,36 @@
       </c>
       <c r="C3">
         <v>43</v>
+      </c>
+      <c r="D3">
+        <v>8996</v>
+      </c>
+      <c r="E3">
+        <v>8996</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>7.47</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>7.27</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>0.44</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0.19</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -3648,6 +3708,36 @@
       <c r="C4">
         <v>32</v>
       </c>
+      <c r="D4">
+        <v>10115</v>
+      </c>
+      <c r="E4">
+        <v>10115</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>6.45</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>6.25</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>0.26</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -3659,6 +3749,36 @@
       <c r="C5">
         <v>3</v>
       </c>
+      <c r="D5">
+        <v>4276</v>
+      </c>
+      <c r="E5">
+        <v>4276</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>61.28</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>61</v>
+      </c>
+      <c r="J5">
+        <v>1266</v>
+      </c>
+      <c r="K5">
+        <v>32.11</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -3670,6 +3790,36 @@
       <c r="C6">
         <v>63</v>
       </c>
+      <c r="D6">
+        <v>11382</v>
+      </c>
+      <c r="E6">
+        <v>11382</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>10.91</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>10.67</v>
+      </c>
+      <c r="J6">
+        <v>28</v>
+      </c>
+      <c r="K6">
+        <v>3.12</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>1.07</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -3681,6 +3831,36 @@
       <c r="C7">
         <v>3</v>
       </c>
+      <c r="D7">
+        <v>8874</v>
+      </c>
+      <c r="E7">
+        <v>8874</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>12.31</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>12.04</v>
+      </c>
+      <c r="J7">
+        <v>52</v>
+      </c>
+      <c r="K7">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="L7">
+        <v>21</v>
+      </c>
+      <c r="M7">
+        <v>2.0099999999999998</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -3692,6 +3872,36 @@
       <c r="C8">
         <v>18</v>
       </c>
+      <c r="D8">
+        <v>13643</v>
+      </c>
+      <c r="E8">
+        <v>13643</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>11.11</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>10.88</v>
+      </c>
+      <c r="J8">
+        <v>33</v>
+      </c>
+      <c r="K8">
+        <v>2.54</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>0.87</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -3703,6 +3913,36 @@
       <c r="C9">
         <v>61</v>
       </c>
+      <c r="D9">
+        <v>13439</v>
+      </c>
+      <c r="E9">
+        <v>13439</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>11.37</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>11.13</v>
+      </c>
+      <c r="J9">
+        <v>18</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -3714,6 +3954,36 @@
       <c r="C10">
         <v>12</v>
       </c>
+      <c r="D10">
+        <v>14488</v>
+      </c>
+      <c r="E10">
+        <v>14488</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>10.6</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>10.42</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>0.99</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -3725,6 +3995,36 @@
       <c r="C11">
         <v>54</v>
       </c>
+      <c r="D11">
+        <v>11862</v>
+      </c>
+      <c r="E11">
+        <v>11862</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="J11">
+        <v>99</v>
+      </c>
+      <c r="K11">
+        <v>7.7</v>
+      </c>
+      <c r="L11">
+        <v>32</v>
+      </c>
+      <c r="M11">
+        <v>2.5499999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -3736,6 +4036,36 @@
       <c r="C12">
         <v>6</v>
       </c>
+      <c r="D12">
+        <v>14349</v>
+      </c>
+      <c r="E12">
+        <v>14349</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>10.89</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>10.52</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>2.5</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -3747,6 +4077,36 @@
       <c r="C13">
         <v>26</v>
       </c>
+      <c r="D13">
+        <v>11159</v>
+      </c>
+      <c r="E13">
+        <v>11159</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>16.89</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>16.64</v>
+      </c>
+      <c r="J13">
+        <v>79</v>
+      </c>
+      <c r="K13">
+        <v>7.42</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>1.01</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -3758,6 +4118,36 @@
       <c r="C14">
         <v>12</v>
       </c>
+      <c r="D14">
+        <v>14488</v>
+      </c>
+      <c r="E14">
+        <v>14488</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>8.06</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>7.78</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>0.3</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -3769,6 +4159,36 @@
       <c r="C15">
         <v>69</v>
       </c>
+      <c r="D15">
+        <v>7813</v>
+      </c>
+      <c r="E15">
+        <v>7813</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>39.44</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>39.25</v>
+      </c>
+      <c r="J15">
+        <v>231</v>
+      </c>
+      <c r="K15">
+        <v>11.64</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -3780,8 +4200,38 @@
       <c r="C16">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>8107</v>
+      </c>
+      <c r="E16">
+        <v>8107</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>9.69</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>9.34</v>
+      </c>
+      <c r="J16">
+        <v>13</v>
+      </c>
+      <c r="K16">
+        <v>1.23</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3791,8 +4241,38 @@
       <c r="C17">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>5419</v>
+      </c>
+      <c r="E17">
+        <v>5419</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>96.37</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>96.07</v>
+      </c>
+      <c r="J17">
+        <v>575</v>
+      </c>
+      <c r="K17">
+        <v>21.97</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3802,8 +4282,38 @@
       <c r="C18">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>5774</v>
+      </c>
+      <c r="E18">
+        <v>5774</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>84.21</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>83.84</v>
+      </c>
+      <c r="J18">
+        <v>1782</v>
+      </c>
+      <c r="K18">
+        <v>50.25</v>
+      </c>
+      <c r="L18">
+        <v>15</v>
+      </c>
+      <c r="M18">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3813,8 +4323,38 @@
       <c r="C19">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <v>14393</v>
+      </c>
+      <c r="E19">
+        <v>14393</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>9.48</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>9.24</v>
+      </c>
+      <c r="J19">
+        <v>9</v>
+      </c>
+      <c r="K19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3824,8 +4364,38 @@
       <c r="C20">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>11382</v>
+      </c>
+      <c r="E20">
+        <v>11382</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>13.19</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>12.96</v>
+      </c>
+      <c r="J20">
+        <v>29</v>
+      </c>
+      <c r="K20">
+        <v>3.5</v>
+      </c>
+      <c r="L20">
+        <v>12</v>
+      </c>
+      <c r="M20">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3835,8 +4405,38 @@
       <c r="C21">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <v>16318</v>
+      </c>
+      <c r="E21">
+        <v>16318</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>8.89</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>8.67</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>0.32</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3846,8 +4446,38 @@
       <c r="C22">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <v>13368</v>
+      </c>
+      <c r="E22">
+        <v>13368</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>45.95</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>45.73</v>
+      </c>
+      <c r="J22">
+        <v>230</v>
+      </c>
+      <c r="K22">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="L22">
+        <v>206</v>
+      </c>
+      <c r="M22">
+        <v>14.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3857,8 +4487,38 @@
       <c r="C23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23">
+        <v>10599</v>
+      </c>
+      <c r="E23">
+        <v>10599</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>8.34</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>8.14</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="K23">
+        <v>0.73</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3868,8 +4528,38 @@
       <c r="C24">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24">
+        <v>10171</v>
+      </c>
+      <c r="E24">
+        <v>10171</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>30.14</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>29.88</v>
+      </c>
+      <c r="J24">
+        <v>86</v>
+      </c>
+      <c r="K24">
+        <v>6.48</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3879,8 +4569,38 @@
       <c r="C25">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <v>12839</v>
+      </c>
+      <c r="E25">
+        <v>12839</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>11.55</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>11.26</v>
+      </c>
+      <c r="J25">
+        <v>21</v>
+      </c>
+      <c r="K25">
+        <v>2.35</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3890,8 +4610,38 @@
       <c r="C26">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26">
+        <v>12184</v>
+      </c>
+      <c r="E26">
+        <v>12184</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>12.85</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>12.54</v>
+      </c>
+      <c r="J26">
+        <v>23</v>
+      </c>
+      <c r="K26">
+        <v>2.87</v>
+      </c>
+      <c r="L26">
+        <v>10</v>
+      </c>
+      <c r="M26">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3901,8 +4651,38 @@
       <c r="C27">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27">
+        <v>1995</v>
+      </c>
+      <c r="E27">
+        <v>1995</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>16.36</v>
+      </c>
+      <c r="J27">
+        <v>399</v>
+      </c>
+      <c r="K27">
+        <v>6.01</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3912,8 +4692,38 @@
       <c r="C28">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <v>11025</v>
+      </c>
+      <c r="E28">
+        <v>11025</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>18.79</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <v>18.47</v>
+      </c>
+      <c r="J28">
+        <v>41</v>
+      </c>
+      <c r="K28">
+        <v>8.52</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3923,8 +4733,38 @@
       <c r="C29">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>14393</v>
+      </c>
+      <c r="E29">
+        <v>14393</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>10.19</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>9.91</v>
+      </c>
+      <c r="J29">
+        <v>9</v>
+      </c>
+      <c r="K29">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3934,8 +4774,38 @@
       <c r="C30">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <v>13090</v>
+      </c>
+      <c r="E30">
+        <v>13090</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>14.38</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>14.15</v>
+      </c>
+      <c r="J30">
+        <v>17</v>
+      </c>
+      <c r="K30">
+        <v>4.46</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
+      </c>
+      <c r="M30">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3945,8 +4815,38 @@
       <c r="C31">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <v>4713</v>
+      </c>
+      <c r="E31">
+        <v>4713</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>40.75</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>40.49</v>
+      </c>
+      <c r="J31">
+        <v>477</v>
+      </c>
+      <c r="K31">
+        <v>17.71</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3956,8 +4856,38 @@
       <c r="C32">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <v>13302</v>
+      </c>
+      <c r="E32">
+        <v>13302</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>13.91</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>13.56</v>
+      </c>
+      <c r="J32">
+        <v>46</v>
+      </c>
+      <c r="K32">
+        <v>4.2</v>
+      </c>
+      <c r="L32">
+        <v>3</v>
+      </c>
+      <c r="M32">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3967,8 +4897,38 @@
       <c r="C33">
         <v>89</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <v>8107</v>
+      </c>
+      <c r="E33">
+        <v>8107</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>10.5</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>10.15</v>
+      </c>
+      <c r="J33">
+        <v>13</v>
+      </c>
+      <c r="K33">
+        <v>1.35</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3978,8 +4938,38 @@
       <c r="C34">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <v>10963</v>
+      </c>
+      <c r="E34">
+        <v>10963</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>16.21</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>15.89</v>
+      </c>
+      <c r="J34">
+        <v>48</v>
+      </c>
+      <c r="K34">
+        <v>6.26</v>
+      </c>
+      <c r="L34">
+        <v>15</v>
+      </c>
+      <c r="M34">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3989,8 +4979,38 @@
       <c r="C35">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35">
+        <v>10840</v>
+      </c>
+      <c r="E35">
+        <v>10840</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>20.79</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>20.54</v>
+      </c>
+      <c r="J35">
+        <v>97</v>
+      </c>
+      <c r="K35">
+        <v>6.1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4000,8 +5020,38 @@
       <c r="C36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <v>11846</v>
+      </c>
+      <c r="E36">
+        <v>11846</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>11.24</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>11.08</v>
+      </c>
+      <c r="J36">
+        <v>28</v>
+      </c>
+      <c r="K36">
+        <v>2.69</v>
+      </c>
+      <c r="L36">
+        <v>17</v>
+      </c>
+      <c r="M36">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4011,8 +5061,38 @@
       <c r="C37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <v>12473</v>
+      </c>
+      <c r="E37">
+        <v>12473</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>6.65</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>6.5</v>
+      </c>
+      <c r="J37">
+        <v>19</v>
+      </c>
+      <c r="K37">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4022,8 +5102,38 @@
       <c r="C38">
         <v>77</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <v>12947</v>
+      </c>
+      <c r="E38">
+        <v>12947</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>10.98</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>10.78</v>
+      </c>
+      <c r="J38">
+        <v>36</v>
+      </c>
+      <c r="K38">
+        <v>2.67</v>
+      </c>
+      <c r="L38">
+        <v>4</v>
+      </c>
+      <c r="M38">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4033,8 +5143,38 @@
       <c r="C39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <v>14632</v>
+      </c>
+      <c r="E39">
+        <v>14632</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>9.35</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>9.09</v>
+      </c>
+      <c r="J39">
+        <v>10</v>
+      </c>
+      <c r="K39">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4044,8 +5184,38 @@
       <c r="C40">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <v>9841</v>
+      </c>
+      <c r="E40">
+        <v>9841</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40">
+        <v>0.59</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4055,8 +5225,38 @@
       <c r="C41">
         <v>71</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <v>13285</v>
+      </c>
+      <c r="E41">
+        <v>13285</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>10.96</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>10.76</v>
+      </c>
+      <c r="J41">
+        <v>26</v>
+      </c>
+      <c r="K41">
+        <v>2.59</v>
+      </c>
+      <c r="L41">
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4066,8 +5266,38 @@
       <c r="C42">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42">
+        <v>7352</v>
+      </c>
+      <c r="E42">
+        <v>7352</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>68.959999999999994</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>68.75</v>
+      </c>
+      <c r="J42">
+        <v>486</v>
+      </c>
+      <c r="K42">
+        <v>22.25</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4077,8 +5307,38 @@
       <c r="C43">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <v>12396</v>
+      </c>
+      <c r="E43">
+        <v>12396</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>12.61</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>12.36</v>
+      </c>
+      <c r="J43">
+        <v>30</v>
+      </c>
+      <c r="K43">
+        <v>3.76</v>
+      </c>
+      <c r="L43">
+        <v>8</v>
+      </c>
+      <c r="M43">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4088,8 +5348,38 @@
       <c r="C44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44">
+        <v>12562</v>
+      </c>
+      <c r="E44">
+        <v>12562</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>9.11</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="J44">
+        <v>10</v>
+      </c>
+      <c r="K44">
+        <v>0.93</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4099,8 +5389,38 @@
       <c r="C45">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45">
+        <v>13882</v>
+      </c>
+      <c r="E45">
+        <v>13882</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>8.59</v>
+      </c>
+      <c r="J45">
+        <v>28</v>
+      </c>
+      <c r="K45">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="L45">
+        <v>7</v>
+      </c>
+      <c r="M45">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4110,8 +5430,38 @@
       <c r="C46">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46">
+        <v>9788</v>
+      </c>
+      <c r="E46">
+        <v>9788</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>22.35</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>22.17</v>
+      </c>
+      <c r="J46">
+        <v>399</v>
+      </c>
+      <c r="K46">
+        <v>15.46</v>
+      </c>
+      <c r="L46">
+        <v>64</v>
+      </c>
+      <c r="M46">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4121,8 +5471,38 @@
       <c r="C47">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47">
+        <v>6852</v>
+      </c>
+      <c r="E47">
+        <v>6852</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>7.34</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>7.19</v>
+      </c>
+      <c r="J47">
+        <v>22</v>
+      </c>
+      <c r="K47">
+        <v>1.18</v>
+      </c>
+      <c r="L47">
+        <v>12</v>
+      </c>
+      <c r="M47">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4132,8 +5512,38 @@
       <c r="C48">
         <v>71</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D48">
+        <v>10485</v>
+      </c>
+      <c r="E48">
+        <v>10485</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>11.72</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>11.22</v>
+      </c>
+      <c r="J48">
+        <v>23</v>
+      </c>
+      <c r="K48">
+        <v>3.01</v>
+      </c>
+      <c r="L48">
+        <v>2</v>
+      </c>
+      <c r="M48">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4143,8 +5553,38 @@
       <c r="C49">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D49">
+        <v>9901</v>
+      </c>
+      <c r="E49">
+        <v>9901</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>23.78</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>23.51</v>
+      </c>
+      <c r="J49">
+        <v>107</v>
+      </c>
+      <c r="K49">
+        <v>6.16</v>
+      </c>
+      <c r="L49">
+        <v>2</v>
+      </c>
+      <c r="M49">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4154,8 +5594,38 @@
       <c r="C50">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D50">
+        <v>12595</v>
+      </c>
+      <c r="E50">
+        <v>12595</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>14.68</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>14.45</v>
+      </c>
+      <c r="J50">
+        <v>36</v>
+      </c>
+      <c r="K50">
+        <v>6.31</v>
+      </c>
+      <c r="L50">
+        <v>3</v>
+      </c>
+      <c r="M50">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4165,41 +5635,71 @@
       <c r="C51">
         <v>74</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D51">
+        <v>11025</v>
+      </c>
+      <c r="E51">
+        <v>11025</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>14.72</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>14.44</v>
+      </c>
+      <c r="J51">
+        <v>41</v>
+      </c>
+      <c r="K51">
+        <v>5.49</v>
+      </c>
+      <c r="L51">
+        <v>4</v>
+      </c>
+      <c r="M51">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D54" t="s">
         <v>13</v>
       </c>
-      <c r="E54" t="e">
+      <c r="E54">
         <f>AVERAGE(E2:E51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+        <v>10976.32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D55" t="s">
         <v>14</v>
       </c>
       <c r="E55">
         <f>MAX(E2:E51)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+        <v>16318</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D56" t="s">
         <v>15</v>
       </c>
       <c r="E56">
         <f>MIN(E2:E51)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D57" t="s">
         <v>16</v>
       </c>
-      <c r="E57" t="e">
+      <c r="E57">
         <f>_xlfn.STDEV.P(E2:E51)</f>
-        <v>#DIV/0!</v>
+        <v>3038.8935120533592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>